<commit_message>
Signin - initial screen validations
</commit_message>
<xml_diff>
--- a/src/main/java/resources/Cantaloupe.xlsx
+++ b/src/main/java/resources/Cantaloupe.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5CCA97-FD4B-9B4B-81BB-2566839E3A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17DE6500-B3A3-034E-AE35-D1B1184EC1B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -175,9 +175,6 @@
     <t>cntlp3@yopmail.com</t>
   </si>
   <si>
-    <t>shahdab.banday26@gmail.com</t>
-  </si>
-  <si>
     <t>wrongPassword</t>
   </si>
   <si>
@@ -191,6 +188,9 @@
   </si>
   <si>
     <t>2398 williamns town</t>
+  </si>
+  <si>
+    <t>shahdab.banday26+58@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -571,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DEB5F1-9A58-E643-A3E3-F7969599581F}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -652,12 +652,12 @@
         <v>24</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>44</v>
@@ -666,22 +666,22 @@
         <v>48</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
         <v>28</v>
       </c>
       <c r="G2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H2">
         <v>1234567894</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>15</v>
@@ -717,7 +717,7 @@
         <v>45040</v>
       </c>
       <c r="U2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed Data Provider - Added Final Constants
</commit_message>
<xml_diff>
--- a/src/main/java/resources/Cantaloupe.xlsx
+++ b/src/main/java/resources/Cantaloupe.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4A5D5F-5AA8-9044-B489-7F05B85195C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F4DFA5-754F-9346-BFE7-DAFCA5A22788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -572,7 +572,7 @@
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>